<commit_message>
Update 4i field descriptions
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="4i" r:id="rId3" sheetId="1"/>
+    <sheet name="4i (Iterative Indirect Immunofl" r:id="rId3" sheetId="1"/>
     <sheet name="dataset_type" r:id="rId4" sheetId="2"/>
     <sheet name="analyte_class" r:id="rId5" sheetId="3"/>
     <sheet name="is_targeted" r:id="rId6" sheetId="4"/>
@@ -28,189 +28,199 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"/TEST001-RK/" for this field. If there are multiple directory levels, use the
-format "/TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) This is the location of the antibodies.tsv file relative to the root
-of the top level of the upload directory structure. This path should begin with
-"." and would likely be something like "./extras/antibodies.tsv".</t>
+        <t>(Required) The path to the antibodies.tsv file relative to the root directory of
+the upload structure. This path should start with "." and is typically formatted
+as "./extras/antibodies.tsv". Example: ./extras/antibodies.tsv</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) Number of antibodies</t>
+        <t>(Required) The number of antibodies used in the assay. If no antibodies were
+utilized, enter 0. Example: 5</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) Number of fluorescent channels imaged during each cycle.</t>
+        <t>(Required) The number of fluorescent channels that are imaged during each cycle.
+Example: 3</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) Number of imaging rounds to capture the tagged biomarkers. For CODEX
-a biomarker imaging round consists of 1. oligo and fluor application, 2.
-imaging, 3. removal of oligo and fluor along washes. For Cell DIVE a biomarker
-imaging round consists of 1. staining of a biomarker via secondary detection or
-direct conjugate and 2. dye inactivation.</t>
+        <t>(Required) The number of imaging rounds required to capture the tagged
+biomarkers. For CODEX, a biomarker imaging round includes steps such as (1)
+oligo application, (2) fluor application, and (3) washes. For Cell DIVE, it
+involves (1) the staining of a biomarker via secondary detection or direct
+conjugate, followed by (2) dye inactivation. Example: 3</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>(Required) The total number of acquisitions performed on microscope to collect
-autofluorescence/background or stained signal (e.g., histology).</t>
+        <t>(Required) The total number of imaging rounds performed using a microscope to
+collect either autofluorescence/background or stained signals, such as those
+used in histological analysis. Example: 5</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>(Required) A unique ID denoting the slide used. This allows users the ability to
+        <t>(Required) The unique identifier assigned to each slide, enabling users to
 determine which tissue sections were processed together on the same slide. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+recommended that data providers prefix the ID with the center name to prevent
+overlapping values across different centers. Example: VAN0071-PA-1-1_AF</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>If a marker or stain was used to identify all cell boundaries in the tissue,
-then the name of the marker or stain should be included here. The name of the
-antibody-targeted molecule marker or non-antibody targeted molecule stain
-included here must be identical to what is found in the imaging data. For
-example, with the PhenoCycler, this name must match the value found in the XPD
-output file. If multiple marker or stains are used to identify all cell
-boundaries, then a comma separated list should be used here.</t>
+        <t>The name of the marker or stain used to identify all cell boundaries in the
+tissue. This name must exactly match the antibody-targeted molecule marker or
+non-antibody targeted molecule stain as found in the imaging data. For example,
+in the case of using the PhenoCycler, ensure the name corresponds to the value
+in the XPD output file. If multiple markers or stains are employed, list them in
+a comma-separated format. Example: Pan-Cytokeratin, E-Cadherin</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>For markers, an antibody-targetted molecule present in or around the cell
-nucleus, the protein or gene symbol that identifies the antibody target that is
-used as the nuclear marker. This symbol must match the antibody target that is
-either generated from the panel used or entered with custom panels. Preferably,
-if using a custom antibody marker, this symbol should be the HGNC symbol
-(https://www.genenames.org/).   For non-protein targets this is the stain name
-(e.g., DAPI) and, when appropriate, associated staining kit and vendor. For the
-PhenoCycler, this symbol must match the value found in the XPD output file.</t>
+        <t>The nuclear marker or stain used, which can be an antibody-targeted molecule
+present in or around the cell nucleus. For protein targets, use the protein or
+gene symbol that identifies the antibody target, ensuring it matches the
+antibody target from the panel used or custom panels. Preferably, if using a
+custom antibody marker, this symbol should be the HGNC symbol
+(https://www.genenames.org/). For non-protein targets, provide the stain name
+(e.g., DAPI) and, when applicable, include the associated staining kit and
+vendor. For the PhenoCycler, ensure the symbol matches the value found in the
+XPD output file. Example: DAPI</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+        <t>Specifies a semicolon-separated list of non-global files that are to be included
+in the dataset. The file paths assume that the files are located in the
+"TOP/non-global/" directory. For instance, if the file is located at
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson, the value for
+this field would be "./lab_processed/images/1-tissue-boundary.geojson". Once
+ingested, these files will be copied to their appropriate locations within the
+respective dataset directory tree. This field is intended for internal HuBMAP
+processing. Examples for GeoMx and PhenoCycler are provided in the File
+Locations documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee
+Example: ./lab_processed/images/1-tissue-boundary.geojson</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -219,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="386">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -239,48 +249,168 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>SNARE-seq2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
     <t>Olink</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
   </si>
   <si>
-    <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
-  </si>
-  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
-  </si>
-  <si>
     <t>FACS</t>
   </si>
   <si>
@@ -293,42 +423,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -359,16 +453,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -377,30 +465,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -431,18 +501,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -455,18 +513,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>Pixel-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000449</t>
-  </si>
-  <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -479,42 +525,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>4i</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
-  </si>
-  <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
-  </si>
-  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -1169,6 +1185,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1199,6 +1218,12 @@
     <t>https://identifiers.org/RRID:SCR_027095</t>
   </si>
   <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1343,6 +1368,9 @@
     <t>schema:title</t>
   </si>
   <si>
+    <t>4i (Iterative Indirect Immunofluorescence Imaging)</t>
+  </si>
+  <si>
     <t>pav:version</t>
   </si>
   <si>
@@ -1352,7 +1380,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-07-24T21:14:17-07:00</t>
+    <t>2025-10-09T11:15:29-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1496,78 +1524,78 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$48</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1579,7 +1607,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$75</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1620,7 +1648,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2008,6 +2036,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2025,130 +2061,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2166,12 +2202,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2189,242 +2225,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2434,7 +2470,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2442,602 +2478,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>316</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>167</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>168</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>322</v>
+        <v>169</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>323</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>345</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3055,42 +3107,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3108,26 +3160,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3143,7 +3195,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.20703125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.65234375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="69.76171875" customWidth="true" bestFit="true"/>
@@ -3151,30 +3203,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>86</v>
+        <v>379</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update MxFBE metadata templates to use updated field descriptions
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="388">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -255,6 +255,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
     <t>Visium (no probes)</t>
   </si>
   <si>
@@ -1380,7 +1386,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-09T11:15:29-07:00</t>
+    <t>2025-10-17T13:44:31-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1524,78 +1530,78 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$49</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1648,7 +1654,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2044,6 +2050,14 @@
       </c>
       <c r="B49" t="s" s="0">
         <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2061,130 +2075,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2202,12 +2216,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2225,242 +2239,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2478,618 +2492,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3107,42 +3121,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3160,26 +3174,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3203,30 +3217,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "RNA + protein" as a new analyte class
Closes #130
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="390">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -297,6 +297,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
+    <t>Virtual Histology</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000473</t>
+  </si>
+  <si>
     <t>DBiT-seq</t>
   </si>
   <si>
@@ -552,18 +558,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
   </si>
   <si>
-    <t>Nucleic acid + protein</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000273</t>
-  </si>
-  <si>
     <t>Chromatin</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>RNA + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000474</t>
+  </si>
+  <si>
     <t>RNA</t>
   </si>
   <si>
@@ -1386,7 +1392,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-17T13:44:31-07:00</t>
+    <t>2025-11-19T14:38:32-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1530,78 +1536,78 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$50</formula1>
+      <formula1>'dataset_type'!$A$1:$A$51</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1654,7 +1660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2058,6 +2064,14 @@
       </c>
       <c r="B50" t="s" s="0">
         <v>103</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2075,130 +2089,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2216,12 +2230,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2239,242 +2253,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2492,618 +2506,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3121,42 +3135,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3174,26 +3188,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3217,30 +3231,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added back Nucleic acid + protein as analyte class
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="392">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -558,6 +558,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
   </si>
   <si>
+    <t>Nucleic acid + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000273</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -1392,7 +1398,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-19T14:38:32-08:00</t>
+    <t>2025-11-20T09:39:32-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1539,61 +1545,61 @@
         <v>106</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2">
@@ -1601,7 +1607,7 @@
         <v>48</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1616,7 @@
       <formula1>'dataset_type'!$A$1:$A$51</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$16</formula1>
+      <formula1>'analyte_class'!$A$1:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
@@ -2081,7 +2087,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2213,6 +2219,14 @@
       </c>
       <c r="B16" t="s" s="0">
         <v>138</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2230,12 +2244,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2253,242 +2267,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2506,474 +2520,474 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60">
@@ -2981,143 +2995,143 @@
         <v>70</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3135,42 +3149,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3188,26 +3202,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3231,30 +3245,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Add Revvity and Opera Phenix Plus HCS for the acquisition instrument
Closes #136

The instrument model is registered as "Opera Phenix Plus HCS"
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="406">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -531,6 +531,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
   </si>
   <si>
+    <t>Raman Imaging</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000475</t>
+  </si>
+  <si>
     <t>RNAseq (with probes)</t>
   </si>
   <si>
@@ -543,6 +549,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
+    <t>STARmap</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000476</t>
+  </si>
+  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -816,6 +828,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -945,6 +963,12 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -987,6 +1011,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1113,6 +1143,12 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1254,6 +1290,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -1398,7 +1440,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-20T09:39:32-08:00</t>
+    <t>2025-12-15T11:28:13-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1542,64 +1584,64 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>382</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2">
@@ -1607,13 +1649,13 @@
         <v>48</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>383</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$51</formula1>
+      <formula1>'dataset_type'!$A$1:$A$53</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$17</formula1>
@@ -1622,10 +1664,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$81</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1666,7 +1708,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2078,6 +2120,22 @@
       </c>
       <c r="B51" t="s" s="0">
         <v>105</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2095,138 +2153,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2244,12 +2302,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2259,7 +2317,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2267,242 +2325,250 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2512,7 +2578,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2520,618 +2586,650 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>70</v>
+        <v>330</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>328</v>
+        <v>335</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>329</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>175</v>
+        <v>337</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>335</v>
+        <v>179</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>336</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>356</v>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -3149,42 +3247,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>368</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3202,26 +3300,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>364</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3245,30 +3343,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>391</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Added new acquisition instrument models
Closes #136, #137
</commit_message>
<xml_diff>
--- a/4i/latest/4i.xlsx
+++ b/4i/latest/4i.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="412">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -768,6 +768,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -963,6 +969,12 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
     <t>Opera Phenix Plus HCS</t>
   </si>
   <si>
@@ -1143,6 +1155,12 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
     <t>Zeiss LightSheet Z.1</t>
   </si>
   <si>
@@ -1440,7 +1458,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-12-15T11:28:13-08:00</t>
+    <t>2025-12-17T13:03:02-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1593,55 +1611,55 @@
         <v>148</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2">
@@ -1649,7 +1667,7 @@
         <v>48</v>
       </c>
       <c r="X2" t="s" s="25">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -1664,10 +1682,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$31</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$32</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$81</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$83</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2317,7 +2335,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2571,6 +2589,14 @@
         <v>210</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2578,7 +2604,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2586,650 +2612,666 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>70</v>
+        <v>338</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>339</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>179</v>
+        <v>345</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>180</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>345</v>
+        <v>181</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>346</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="0">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -3247,42 +3289,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3300,26 +3342,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -3343,30 +3385,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>405</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>